<commit_message>
Non Windows tests expectaion fix
* Dropped pre net standard os detection code
* Fix -test expectation on systems without the fonts used to create expectation
* Fix - If a width of consecutive column gets calced to an equal value the style description gets combined - that was not expected by the test infrastructure
* Fix - MiscTests.AdjustToContents - the height differs depending on the avaliable font set
* Fix - some tests that rely on english exception messages
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Tables/ResizingTables.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Tables/ResizingTables.xlsx
@@ -511,10 +511,10 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.400625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="12.875425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="11.880625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="10.685425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="12.090625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="11.335425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.940625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="9.405425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:5">
@@ -702,10 +702,10 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.400625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="12.875425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="11.880625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="10.685425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="12.090625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="11.335425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.940625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="9.405425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:5">
@@ -899,11 +899,11 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="12.195425" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.400625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="12.875425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="11.880625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="10.685425" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="10.795425" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="12.090625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="11.335425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.940625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="9.405425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:5">
@@ -1101,11 +1101,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.400625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="12.875425" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="11.880625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="12.090625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="11.335425" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.940625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="10.685425" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="9.405425" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>